<commit_message>
Go through 04 script with just Sonoran
</commit_message>
<xml_diff>
--- a/Sonoran-data/data-wrangling-intermediate/01b_edited7_location-dependent-final-fix.xlsx
+++ b/Sonoran-data/data-wrangling-intermediate/01b_edited7_location-dependent-final-fix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/Sonoran-data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{C3EF6CDF-594F-4BE4-9EF4-7E0609E88FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46A1F7FA-89F8-4F57-85D1-42C04A64250A}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{C3EF6CDF-594F-4BE4-9EF4-7E0609E88FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E5F93CD-B058-4F53-B5BC-F9320D6E5DDF}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{A09795D3-E60D-44CB-9C72-087875526995}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{A09795D3-E60D-44CB-9C72-087875526995}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -961,7 +961,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>Changed cells are highlighted. Changed native status when cross-referencing master species list for unknowns.</a:t>
+            <a:t>Changed cells are highlighted. Changed native status when cross-referencing master species list for unknowns. Switched names between Patagonia &amp; SRER when specified in name.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -970,10 +970,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1295,15 +1291,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6595BD7-2435-430D-9E63-650FB0A0F724}">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="16.21875" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" customWidth="1"/>
-    <col min="5" max="5" width="20.77734375" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="39.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -1865,8 +1861,8 @@
       <c r="D22" t="s">
         <v>102</v>
       </c>
-      <c r="E22" t="s">
-        <v>105</v>
+      <c r="E22" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="F22" t="s">
         <v>14</v>
@@ -2827,8 +2823,8 @@
       <c r="D59" t="s">
         <v>102</v>
       </c>
-      <c r="E59" t="s">
-        <v>103</v>
+      <c r="E59" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="F59" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Rerun 01.R Sonoran script. Update README and make small changes to output/edited2 and output/edited5, but final clean data does not change.
</commit_message>
<xml_diff>
--- a/Sonoran-data/data-wrangling-intermediate/01b_edited7_location-dependent-final-fix.xlsx
+++ b/Sonoran-data/data-wrangling-intermediate/01b_edited7_location-dependent-final-fix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/Sonoran-data/data-wrangling-intermediate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eltnmsu-my.sharepoint.com/personal/lossanna_nmsu_edu/Documents/Documents/02_RestoreNet/RestoreNet/Sonoran-data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{C3EF6CDF-594F-4BE4-9EF4-7E0609E88FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E5F93CD-B058-4F53-B5BC-F9320D6E5DDF}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{C3EF6CDF-594F-4BE4-9EF4-7E0609E88FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDDD24C0-60DD-42AC-BD14-8F9884CBB6E0}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{A09795D3-E60D-44CB-9C72-087875526995}"/>
+    <workbookView xWindow="12495" yWindow="0" windowWidth="12810" windowHeight="15135" xr2:uid="{A09795D3-E60D-44CB-9C72-087875526995}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -961,7 +961,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>Changed cells are highlighted. Changed native status when cross-referencing master species list for unknowns. Switched names between Patagonia &amp; SRER when specified in name.</a:t>
+            <a:t>Changed cells are highlighted. Changed native status based on details in name. Switched names between Patagonia &amp; SRER when specified in name.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -1291,18 +1291,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6595BD7-2435-430D-9E63-650FB0A0F724}">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.21875" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="39.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="39.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>8</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -2498,7 +2498,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>8</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>8</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>8</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>8</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>8</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>8</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>8</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>8</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>8</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>8</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>8</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>8</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>8</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>8</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -3330,7 +3330,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>8</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>8</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>8</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>8</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>8</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>8</v>
       </c>

</xml_diff>